<commit_message>
Changed the file contents
</commit_message>
<xml_diff>
--- a/Data/TestCoverage.xlsx
+++ b/Data/TestCoverage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdurgam\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdurgam\git\projects\dash\plotlydash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A252A3A3-7A6A-467B-8574-1E7D32203F7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC33EE3-2B0F-4540-9697-BD80F4F1AF4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B087308D-A530-467A-AC78-2C6E763EFCF5}"/>
   </bookViews>
@@ -65,22 +65,22 @@
     <t>TC Blocked</t>
   </si>
   <si>
-    <t>Retailer Location</t>
-  </si>
-  <si>
-    <t>Anywhere Random</t>
-  </si>
-  <si>
-    <t>Ticket Inquiry (Draw Games)</t>
-  </si>
-  <si>
-    <t>Winning Numbers (Draw Games)</t>
-  </si>
-  <si>
-    <t>Ticket Inquiry (Instant Games)</t>
-  </si>
-  <si>
-    <t>Instant Games (Active games)</t>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Ticket Inquire</t>
+  </si>
+  <si>
+    <t>Winnings and Numbers</t>
+  </si>
+  <si>
+    <t>Ticket Inquire Now</t>
+  </si>
+  <si>
+    <t>Next Gen Games</t>
   </si>
 </sst>
 </file>
@@ -133,10 +133,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,7 +435,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12:J13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>